<commit_message>
added slope significance to the plots
</commit_message>
<xml_diff>
--- a/round_6_TeTuSu_UNSCALED/param_tuning_dataframe_1978-2015_TEMP.xlsx
+++ b/round_6_TeTuSu_UNSCALED/param_tuning_dataframe_1978-2015_TEMP.xlsx
@@ -3104,7 +3104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3219,6 +3219,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3264,8 +3303,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3611,8 +3653,8 @@
   <dimension ref="A1:AA190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12329,7 +12371,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -12412,86 +12454,86 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A107">
+    <row r="107" spans="1:27" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
         <v>106</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="3">
         <v>3</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="3">
         <v>405</v>
       </c>
-      <c r="G107">
+      <c r="G107" s="3">
         <v>12353.544131843901</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="1">
         <v>25517.088263687801</v>
       </c>
-      <c r="I107">
+      <c r="I107" s="3">
         <v>0.82285233795559698</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="3">
         <v>0.95783115906998195</v>
       </c>
-      <c r="K107">
+      <c r="K107" s="3">
         <v>0.99252565558738903</v>
       </c>
-      <c r="L107">
+      <c r="L107" s="3">
         <v>7</v>
       </c>
-      <c r="M107">
+      <c r="M107" s="3">
         <v>1</v>
       </c>
-      <c r="N107">
-        <v>0</v>
-      </c>
-      <c r="O107">
-        <v>0</v>
-      </c>
-      <c r="P107" t="s">
+      <c r="N107" s="3">
+        <v>0</v>
+      </c>
+      <c r="O107" s="3">
+        <v>0</v>
+      </c>
+      <c r="P107" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="Q107" t="s">
+      <c r="Q107" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="R107" t="s">
+      <c r="R107" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="S107" t="s">
-        <v>30</v>
-      </c>
-      <c r="T107" t="s">
+      <c r="S107" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T107" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="U107" t="s">
+      <c r="U107" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="V107" t="s">
+      <c r="V107" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="W107" t="s">
-        <v>30</v>
-      </c>
-      <c r="X107" t="s">
+      <c r="W107" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X107" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="Y107" t="s">
-        <v>30</v>
-      </c>
-      <c r="Z107" t="s">
+      <c r="Y107" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z107" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="AA107" t="s">
+      <c r="AA107" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -19386,7 +19428,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H128:H190">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19398,7 +19440,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G128:G190">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19409,6 +19451,66 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I190">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J190">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K190">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G127">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H127">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>